<commit_message>
W3C CSS page accueil
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiengtb/Dropbox/DEVELOPPEMENT/Programmation/01. Développeur Web/Projets OC/Projet 4/damienwill_4_07062021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F0824A-E3A7-0A4C-A908-498C2B0D680D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F4EC4F-F54A-844F-9EF1-E7C06F349F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83460" yWindow="-13160" windowWidth="41440" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-87540" yWindow="-15120" windowWidth="46220" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page accueil" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="214">
   <si>
     <t>Catégorie</t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>Paramétrer l'attribut " lang" du html avec la version fr.</t>
+  </si>
+  <si>
+    <t>Bien pour les sites statiques mais pas pour les dynamiques</t>
   </si>
 </sst>
 </file>
@@ -1158,6 +1161,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1175,39 +1211,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1427,9 +1430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1696,21 +1699,21 @@
       <c r="I9" s="27"/>
     </row>
     <row r="10" spans="1:28" s="56" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="75" t="s">
+      <c r="C10" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="D10" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="E10" s="78" t="s">
+      <c r="E10" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="G10" s="76" t="s">
+      <c r="G10" s="70" t="s">
         <v>107</v>
       </c>
       <c r="H10" s="23" t="s">
@@ -1721,26 +1724,26 @@
       </c>
     </row>
     <row r="11" spans="1:28" s="56" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="77"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
       <c r="H11" s="23" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="22"/>
     </row>
     <row r="12" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="77"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
       <c r="H12" s="23" t="s">
         <v>48</v>
       </c>
@@ -1749,11 +1752,11 @@
     <row r="13" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="76"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="23" t="s">
         <v>102</v>
       </c>
@@ -1762,11 +1765,11 @@
     <row r="14" spans="1:28" s="56" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="71"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
       <c r="H14" s="23" t="s">
         <v>106</v>
       </c>
@@ -1777,11 +1780,11 @@
     <row r="15" spans="1:28" s="56" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
       <c r="H15" s="23" t="s">
         <v>111</v>
       </c>
@@ -1790,20 +1793,20 @@
     <row r="16" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
+      <c r="C16" s="78"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
       <c r="H16" s="23" t="s">
         <v>49</v>
       </c>
       <c r="I16" s="22"/>
     </row>
     <row r="17" spans="1:9" s="56" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="76"/>
+      <c r="A17" s="70"/>
       <c r="B17" s="19"/>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="78" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="14" t="s">
@@ -1815,7 +1818,7 @@
       <c r="F17" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G17" s="84" t="s">
+      <c r="G17" s="77" t="s">
         <v>107</v>
       </c>
       <c r="H17" s="14" t="s">
@@ -1824,9 +1827,9 @@
       <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" s="56" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="77"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="19"/>
-      <c r="C18" s="75"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="14" t="s">
         <v>37</v>
       </c>
@@ -1836,7 +1839,7 @@
       <c r="F18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G18" s="84"/>
+      <c r="G18" s="77"/>
       <c r="H18" s="14" t="s">
         <v>38</v>
       </c>
@@ -1845,15 +1848,17 @@
     <row r="19" spans="1:9" s="56" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
+      <c r="D19" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="E19" s="70"/>
       <c r="F19" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="76"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="23" t="s">
         <v>119</v>
       </c>
@@ -1862,13 +1867,13 @@
     <row r="20" spans="1:9" s="56" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
-      <c r="C20" s="75"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="76"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="21" t="s">
         <v>171</v>
       </c>
@@ -1928,7 +1933,7 @@
       <c r="G23" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H23" s="85" t="s">
+      <c r="H23" s="69" t="s">
         <v>212</v>
       </c>
       <c r="I23" s="67" t="s">
@@ -1963,66 +1968,66 @@
     <row r="25" spans="1:9" s="58" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="80" t="s">
+      <c r="D25" s="73" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="80" t="s">
+      <c r="E25" s="73" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="83" t="s">
+      <c r="G25" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="H25" s="81" t="s">
+      <c r="H25" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="I25" s="79" t="s">
+      <c r="I25" s="72" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="58" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
       <c r="B26" s="35"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
+      <c r="C26" s="78"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
       <c r="F26" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="83"/>
-      <c r="H26" s="82"/>
-      <c r="I26" s="80"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="73"/>
     </row>
     <row r="27" spans="1:9" s="58" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
+      <c r="C27" s="78"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
       <c r="F27" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="G27" s="83"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="80"/>
+      <c r="G27" s="76"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="73"/>
     </row>
     <row r="28" spans="1:9" s="58" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="35"/>
-      <c r="C28" s="75"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
+      <c r="C28" s="78"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="73"/>
       <c r="F28" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="G28" s="83"/>
-      <c r="H28" s="82"/>
-      <c r="I28" s="80"/>
+      <c r="G28" s="76"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="73"/>
     </row>
     <row r="29" spans="1:9" s="58" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
@@ -2299,7 +2304,7 @@
     <row r="41" spans="1:9" s="56" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="19"/>
-      <c r="C41" s="69" t="s">
+      <c r="C41" s="80" t="s">
         <v>149</v>
       </c>
       <c r="D41" s="59" t="s">
@@ -2320,7 +2325,7 @@
     <row r="42" spans="1:9" s="56" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="19"/>
-      <c r="C42" s="69"/>
+      <c r="C42" s="80"/>
       <c r="D42" s="62" t="s">
         <v>201</v>
       </c>
@@ -2339,7 +2344,7 @@
     <row r="43" spans="1:9" s="56" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="69" t="s">
+      <c r="C43" s="80" t="s">
         <v>150</v>
       </c>
       <c r="D43" s="65" t="s">
@@ -2360,7 +2365,7 @@
     <row r="44" spans="1:9" s="56" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="19"/>
-      <c r="C44" s="69"/>
+      <c r="C44" s="80"/>
       <c r="D44" s="60" t="s">
         <v>203</v>
       </c>
@@ -2379,7 +2384,7 @@
     <row r="45" spans="1:9" s="56" customFormat="1" ht="119" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="19"/>
-      <c r="C45" s="70" t="s">
+      <c r="C45" s="81" t="s">
         <v>151</v>
       </c>
       <c r="D45" s="62" t="s">
@@ -2398,7 +2403,7 @@
     <row r="46" spans="1:9" s="56" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="19"/>
-      <c r="C46" s="71"/>
+      <c r="C46" s="82"/>
       <c r="D46" s="62" t="s">
         <v>200</v>
       </c>
@@ -2415,7 +2420,7 @@
     <row r="47" spans="1:9" s="56" customFormat="1" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
-      <c r="C47" s="69" t="s">
+      <c r="C47" s="80" t="s">
         <v>152</v>
       </c>
       <c r="D47" s="60" t="s">
@@ -2434,7 +2439,7 @@
     <row r="48" spans="1:9" s="56" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
-      <c r="C48" s="69"/>
+      <c r="C48" s="80"/>
       <c r="D48" s="65" t="s">
         <v>190</v>
       </c>
@@ -2453,7 +2458,7 @@
     <row r="49" spans="1:9" s="56" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="63"/>
       <c r="B49" s="63"/>
-      <c r="C49" s="69"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="65" t="s">
         <v>184</v>
       </c>
@@ -2472,7 +2477,7 @@
     <row r="50" spans="1:9" s="56" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
-      <c r="C50" s="69"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="65" t="s">
         <v>199</v>
       </c>
@@ -2491,7 +2496,7 @@
     <row r="51" spans="1:9" s="56" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
-      <c r="C51" s="69"/>
+      <c r="C51" s="80"/>
       <c r="D51" s="60" t="s">
         <v>193</v>
       </c>
@@ -2548,7 +2553,7 @@
     <row r="54" spans="1:9" s="56" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="63"/>
       <c r="B54" s="63"/>
-      <c r="C54" s="72" t="s">
+      <c r="C54" s="83" t="s">
         <v>208</v>
       </c>
       <c r="D54" s="65" t="s">
@@ -2565,7 +2570,7 @@
     <row r="55" spans="1:9" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="48"/>
       <c r="B55" s="48"/>
-      <c r="C55" s="73"/>
+      <c r="C55" s="84"/>
       <c r="D55" s="48"/>
       <c r="E55" s="48"/>
       <c r="F55" s="45" t="s">
@@ -2580,7 +2585,7 @@
     <row r="56" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="48"/>
       <c r="B56" s="48"/>
-      <c r="C56" s="74"/>
+      <c r="C56" s="85"/>
       <c r="D56" s="48"/>
       <c r="E56" s="48"/>
       <c r="F56" s="45" t="s">
@@ -2595,7 +2600,7 @@
     <row r="57" spans="1:9" s="56" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
-      <c r="C57" s="69" t="s">
+      <c r="C57" s="80" t="s">
         <v>155</v>
       </c>
       <c r="D57" s="62" t="s">
@@ -2614,7 +2619,7 @@
     <row r="58" spans="1:9" s="56" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="61"/>
       <c r="B58" s="61"/>
-      <c r="C58" s="69"/>
+      <c r="C58" s="80"/>
       <c r="D58" s="59" t="s">
         <v>177</v>
       </c>
@@ -2635,7 +2640,7 @@
     <row r="59" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="48"/>
       <c r="B59" s="48"/>
-      <c r="C59" s="69"/>
+      <c r="C59" s="80"/>
       <c r="D59" s="68" t="s">
         <v>188</v>
       </c>
@@ -2654,7 +2659,7 @@
     <row r="60" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="48"/>
       <c r="B60" s="48"/>
-      <c r="C60" s="69"/>
+      <c r="C60" s="80"/>
       <c r="D60" s="68" t="s">
         <v>196</v>
       </c>
@@ -2673,7 +2678,7 @@
     <row r="61" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="48"/>
       <c r="B61" s="48"/>
-      <c r="C61" s="69"/>
+      <c r="C61" s="80"/>
       <c r="D61" s="68" t="s">
         <v>205</v>
       </c>
@@ -3647,6 +3652,18 @@
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="C57:C61"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C25:C28"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C10:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="D10:D16"/>
     <mergeCell ref="E10:E16"/>
     <mergeCell ref="I25:I28"/>
@@ -3660,18 +3677,6 @@
     <mergeCell ref="G10:G16"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="C10:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="C54:C56"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{B2C3AA74-066E-EE4F-B4DB-D29CC319C308}"/>

</xml_diff>

<commit_message>
description et title page contact
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/damiengtb/Dropbox/DEVELOPPEMENT/Programmation/01. Développeur Web/Projets OC/Projet 4/damienwill_4_07062021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F4EC4F-F54A-844F-9EF1-E7C06F349F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB18CE6-FECF-4F46-9F2A-913E18840C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-87540" yWindow="-15120" windowWidth="46220" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29800" yWindow="-3100" windowWidth="37400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Page accueil" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="216">
   <si>
     <t>Catégorie</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Volume des contenus des pages</t>
   </si>
   <si>
-    <t>Il faut un minimum de 400 mots pour être correctement référencés par Google (certains disent même 1000 mots maintenant !)</t>
-  </si>
-  <si>
     <t>cours SEO Openclassrooms</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">Les url des pages d'accueil et page 2 ne sont pas intelligibles. </t>
-  </si>
-  <si>
-    <t>La vitesse de chargement est acceptable mais peut encore être optimisée</t>
   </si>
   <si>
     <t>Convertir les images dans des formats next-gen comme JPEG 2000, JPEG XR, and WebP</t>
@@ -152,9 +146,6 @@
     <t>Héberger les fonts</t>
   </si>
   <si>
-    <t>L'hebergment des fonts rend leur disponibilité donc le chargement de la page plus rapides.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Les images n'ont pas de paramétrages pour la responsivité, une mauvaise responsivité affecte la crawlabilité du site. </t>
   </si>
   <si>
@@ -180,9 +171,6 @@
   </si>
   <si>
     <t>Attribuer une longue durée de vie du cache peut accélérer les visites répétées sur votre page</t>
-  </si>
-  <si>
-    <t>Hierarchisation des pages</t>
   </si>
   <si>
     <t>La navigation n'informe pas sur les différents contenus par page du site</t>
@@ -237,9 +225,6 @@
     <t>Taille maximum : Google affiche entre 132 et 160 caractères. Il est conseillé d'en écrire un peu plus, pour que Google ait le choix de ce qu'il souhaite afficher.</t>
   </si>
   <si>
-    <t xml:space="preserve">Aidons Google à comprendre le contexte de notre box bio en ajoutant dans la description des mots proches du champs lexical de l'alimentation comme "cuisinez" et "producteurs". </t>
-  </si>
-  <si>
     <t xml:space="preserve">Le mot clé est présent au début de la balise. Nous y rappelons aussi notre nom de marque, nous expliquons au visiteur pourquoi notre box est "la meilleure" et nous présentons ses avantages. </t>
   </si>
   <si>
@@ -290,9 +275,6 @@
     <t>Certains titres ne semblent pas se suivre de manière logique (imbrication logique = h1 puis h2 puis h3 etc.).</t>
   </si>
   <si>
-    <t xml:space="preserve">Une mauvaise structuration des titres va empecher les bots de comprendre la structure de la page et les sujets dont elle traite en priorité. </t>
-  </si>
-  <si>
     <t>Langue</t>
   </si>
   <si>
@@ -318,9 +300,6 @@
   </si>
   <si>
     <t>Cette page comporte 9 image(s) dont le nom ne semble pas optimisé pour le référencement</t>
-  </si>
-  <si>
-    <t>Pour améliorer le référencement de vos images, vous pouvez leur donner un nom explicite dont les mots-clés doivent être séparés par des tirets</t>
   </si>
   <si>
     <t xml:space="preserve">Les mots clés ciblent n'apparaissent pas dans les noms des images et ça ne facilite pas le référencement de ces images. </t>
@@ -330,9 +309,6 @@
 Essayez d'être plus précis dans la rédaction de vos textes alternatifs afin que les moteurs de recherche puissent individualiser vos images</t>
   </si>
   <si>
-    <t>Présents mais pour 3 images il y a du contenu dupliqué</t>
-  </si>
-  <si>
     <t>Les moteurs de recherche ne pourront pas individualiser les images et les référencer correctement</t>
   </si>
   <si>
@@ -340,33 +316,6 @@
   </si>
   <si>
     <t>Donner une width et une height explicites aux images</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-Des images trops lourdes vont ralentir le temps de téléchargement de la page.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
   </si>
   <si>
     <t>Accessibilité</t>
@@ -404,9 +353,6 @@
 </t>
   </si>
   <si>
-    <t>Allèger l'image de favicon</t>
-  </si>
-  <si>
     <t>Créer une sitemap du site</t>
   </si>
   <si>
@@ -417,9 +363,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Il est interprété par les robots en charge du référencement de votre site. Il délivre des instructions pour indiquer les pages à explorer par les robots.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peut être toutes les pages n'auront pas vocation à être indexées. Créer un fichier robots.txt à la racine permet de gérer l'indexation voulue des pages du site </t>
   </si>
   <si>
     <t>Dareboost</t>
@@ -467,9 +410,6 @@
     <t>Remettre un h2 sur page d'accueil</t>
   </si>
   <si>
-    <t>Remplacer les balises div par la bonne nomencalture )main, section, aside, …)</t>
-  </si>
-  <si>
     <t>Renommer les images</t>
   </si>
   <si>
@@ -488,9 +428,6 @@
     <t>La page 2 n'a pas de paragraphe de contenu</t>
   </si>
   <si>
-    <t>SI la page fait moins de 400 mots et si les mots clés ne sont pas représentés, la crwalabilité et le référencement ne seront pas de bonne qualité.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Créer un petit paragraphe expliquant le but de la page. </t>
   </si>
   <si>
@@ -506,9 +443,6 @@
     <t>Si possible, 1 ou 2 liens externes de qualité</t>
   </si>
   <si>
-    <t>Vérifier les lines externes du footer et supprimer ceux qui n'apportent pas de valeur ajoutée</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mettre des mots clés ou titres de pages dans les liens. </t>
   </si>
   <si>
@@ -518,25 +452,13 @@
     <t>W3C</t>
   </si>
   <si>
-    <t>Corriger les erreurs majeurs</t>
-  </si>
-  <si>
     <t>La couleur</t>
   </si>
   <si>
     <t>La visibilité</t>
   </si>
   <si>
-    <t>Le focus</t>
-  </si>
-  <si>
     <t>Les équivalents textuels</t>
-  </si>
-  <si>
-    <t>La gestion des états</t>
-  </si>
-  <si>
-    <t>L'orientation</t>
   </si>
   <si>
     <t>Directives générales</t>
@@ -553,14 +475,6 @@
     Sauf si cela est absolument inévitable, l'attribut aria-hidden NE DOIT PAS être utilisé.</t>
   </si>
   <si>
-    <t>Tous les éléments activables DOIVENT être focusables :
-    Les contrôles standard tels que les liens, les boutons et les champs de formulaire sont accessibles par défaut.
-    Les contrôles non standard DOIVENT avoir un rôle ARIA (en-US) approprié qui leur est attribué, comme button, link ou checkbox.</t>
-  </si>
-  <si>
-    <t>Le focus DOIT être traité dans un ordre logique et de manière cohérente.</t>
-  </si>
-  <si>
     <t>Un équivalent textuel DOIT être fourni pour chaque élément non textuel non strictement présenté dans l'application.
     Utilisez alt et title lorsque cela est approprié (voir l'article de Steve Faulkner sur l'Utilisation de l'attribut HTML title).
     Si les attributs ci-dessus ne sont pas applicables, utilisez les États et propriétés ARIA appropriés tels que aria-label, aria-labelledby, ou aria-describedby.</t>
@@ -570,16 +484,6 @@
   </si>
   <si>
     <t>Tous les contrôles de formulaire DOIVENT avoir des étiquettes (éléments &lt;label&gt;) pour le bénéfice des utilisateurs de lecteurs d'écran.</t>
-  </si>
-  <si>
-    <t>Les contrôles standard tels que les boutons radio et les cases à cocher sont gérés par le système d'exploitation. Cependant, pour d'autres contrôles personnalisés, les changements d'état DOIVENT être fournis via les états ARIA tels que aria-checked, aria-disabled, aria-selected, aria-expanded et aria-pressed.</t>
-  </si>
-  <si>
-    <t>Le contenu NE DOIT PAS être limité à une seule orientation, comme le portrait ou le paysage, sauf si cela est essentiel. WCAG 2.1 : Orientation
-    Des exemples de cas où une orientation est essentielle sont une application pour un piano ou un chèque de banque.</t>
-  </si>
-  <si>
-    <t>Un titre d'application DOIT être fourni.</t>
   </si>
   <si>
     <t>Les titres NE DOIVENT PAS rompre la structure hiérarchique
@@ -589,6 +493,232 @@
     &lt;h3&gt;Titre de bas niveau&lt;/h3&gt;</t>
   </si>
   <si>
+    <t>Paramétrer la durée du cache</t>
+  </si>
+  <si>
+    <t>Des erreurs relevées dans le test W3C</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/</t>
+  </si>
+  <si>
+    <t>Le contraste des couleurs DOIT être conforme aux exigences du niveau AA du WCAG 2.1 :
+    Un contraste dont le ratio est de 4.5:1 pour les textes normaux (dont la font est inférieure à 18 points ou 14 points en gras) ;
+    Un contraste dont le ratio est de 3:1 pour les grands textes (18 points minimum ou 14 points en gras).</t>
+  </si>
+  <si>
+    <t>L'attribut "lang" dans le Html doit être renseigné correctement</t>
+  </si>
+  <si>
+    <t>Lighthouse</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/
+Lighthouse</t>
+  </si>
+  <si>
+    <t>Tous les composants de l'interface utilisateur ayant un texte visible (ou une image de texte) comme étiquette (label) DOIVENT avoir le même texte disponible dans le nom programmatique du composant. WCAG 2.1 : Étiquette dans le nom.</t>
+  </si>
+  <si>
+    <t>Un taux de contraste insuffisant va rendre difficile la lecture pour les personnes mal voyantes.</t>
+  </si>
+  <si>
+    <t>Les éléments interactifs ou cliquables doivent avoir un contenu textuel visible par les lecteurs d'écran</t>
+  </si>
+  <si>
+    <t>Des liens en page 2 n'ont pas de contenu textuel visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le logiciel de lecteur d'écran ne pourra pas restituer à l'utilisateur le contenu et l'intérêt des liens incriminés. </t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/
+Axe Devtools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il existe des images texte en page accueil sans description adaptée. </t>
+  </si>
+  <si>
+    <t>Des contenus textuels sont lus dans un accent anglais, ce qui rend la compréhension difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le remplissage du formulaire par l'utilisateur utilisant une technologie d'assistance risque d'être géné par une mauvaise compréhension des éléments. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">La structure du code html doit utiliser au maximum les balises sémantiques et être cohérente. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de balise main pour les 2 pages. 
+Un bouton "Toggle navigation" semble errer sans but en haut de la page 2. </t>
+  </si>
+  <si>
+    <t>La navigation en page 2 est à moitié hors écran.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cela ne favorise pas la visibilité de la page et la navigation pour les personnes mal voyantes. </t>
+  </si>
+  <si>
+    <t>Des éléments textuels ne sont pas lus par le lecteur d'écran (voice over). Web design, Stratégie, Illustrations + paragraphes associés. 
+Titres et paragraphes des images en page d'accueil. 
+Paragraphes du bouton envoyer en page 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cela risque de rendre difficile la navigation des personnes mal voyantes. </t>
+  </si>
+  <si>
+    <t>Les éléments  dans le footer sont invisibles en page 2</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/
+Ligthouse
+Wave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Axe devtools
+Wave</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/
+WCAG - Contrast checker
+Lighthouse
+Wave</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Paramétrer l'attribut " lang" du html avec la version fr.</t>
+  </si>
+  <si>
+    <t>Changement du background de couleur #F3976C en couleur #f8c3ab</t>
+  </si>
+  <si>
+    <t>Les icônes des réseaux sociaux dans le footer n'ont pas de contenu pouvant être lu par les lecteurs d'écran</t>
+  </si>
+  <si>
+    <t>Renseigner un contenu ou tout du moins un titre.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Il n'y a pas de mise en cache paramétrée pour ce site. </t>
+  </si>
+  <si>
+    <t>Openclassrooms
+Dareboost
+Mentor</t>
+  </si>
+  <si>
+    <t>cours SEO Openclassrooms
+mentor</t>
+  </si>
+  <si>
+    <t>Il faut un minimum de 400 mots pour être correctement référencé par Google (certains disent même 1000 mots maintenant !)</t>
+  </si>
+  <si>
+    <t>Hiérarchisation des pages</t>
+  </si>
+  <si>
+    <t>La vitesse de chargement est acceptable, mais peut encore être optimisée</t>
+  </si>
+  <si>
+    <t>Présents, mais pour 3 images il y a du contenu dupliqué</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Des images trop lourdes vont ralentir le temps de téléchargement de la page.
+</t>
+  </si>
+  <si>
+    <t>Alléger l'image de favicon</t>
+  </si>
+  <si>
+    <t>L'hébergement des fonts rend leur disponibilité donc le chargement de la page plus rapide.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pour un site  statique, la mise en cache de certains éléments par le navigateur peut apporter un gain de vitesse de chargement de la page important. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peut-être toutes les pages n'auront pas vocation à être indexées. Créer un fichier robots.txt à la racine permet de gérer l'indexation voulue des pages du site </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aidons Google à comprendre le contexte de notre box bio en ajoutant dans la description des mots proches du champ lexical de l'alimentation comme "cuisinez" et "producteurs". </t>
+  </si>
+  <si>
+    <t>Remplacer les balises div par la bonne nomenclature )main, section, aside, …)</t>
+  </si>
+  <si>
+    <t>Pour améliorer le référencement de vos images, vous pouvez leur donner un nom explicite dont les mots clés doivent être séparés par des tirets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une mauvaise structuration des titres va empêcher les bots de comprendre la structure de la page et les sujets dont elle traite en priorité. </t>
+  </si>
+  <si>
+    <t>SI la page fait moins de 400 mots et si les mots clés ne sont pas représentés, la crawlabilité et le référencement ne seront pas de bonne qualité.</t>
+  </si>
+  <si>
+    <t>Vérifier les liens externes du footer et supprimer ceux qui n'apportent pas de valeur ajoutée</t>
+  </si>
+  <si>
+    <t>Corriger les erreurs majeures</t>
+  </si>
+  <si>
+    <t>Des parties de pages comportent un ratio de contraste texte/fond insuffisant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les liens du footer en page d'accueil n'ont aucune indication de couleur ou autre (à part le pointer de la souris, mais les liens sont trop rapprochés entre eux pour que ce pointer soit efficace). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le contenu ne pourra pas être lu par un lecteur d'écran ou une technologie d'assistance. L'utilisateur va passer à côté des informations du site. </t>
+  </si>
+  <si>
+    <t>Le formulaire page 2 n'a pas de labels associés. De plus, lors de la lecture d'écran par Voice over, les indications pour chaque input sont identiques.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page d'accueil, la hiérarchie des titres n'est pas correcte. </t>
+  </si>
+  <si>
+    <t>Cela ne facilite pas la compréhension de la page par le lecteur d'écran et les technologies d'assistance.</t>
+  </si>
+  <si>
+    <t>valeur "defaut" définie pour l'attribut "lang" pour les 2 pages</t>
+  </si>
+  <si>
+    <t>Le logiciel de lecteur d'écran ne pourra pas restituer à l'utilisateur le contenu et l'intérêt des textes de la page.</t>
+  </si>
+  <si>
+    <t>Mettre une couleur différente sur le hover du lien, en respectant les normes de contrate.</t>
+  </si>
+  <si>
+    <t>Repositionner+G52 la navigation dans la page</t>
+  </si>
+  <si>
+    <t>Tous les éléments activables DOIVENT être focusables :
+    Les contrôles standard tels que les liens, les boutons et les champs de formulaire sont accessibles par défaut.
+    Les contrôles non standard DOIVENT avoir un rôle ARIA (en-US) approprié qui leur est attribué, comme button, link ou checkbox.</t>
+  </si>
+  <si>
+    <t>Le focus DOIT être traité dans un ordre logique et de manière cohérente.</t>
+  </si>
+  <si>
+    <t>Le focus</t>
+  </si>
+  <si>
+    <t>La gestion des états</t>
+  </si>
+  <si>
+    <t>Les contrôles standard tels que les boutons radio et les cases à cocher sont gérés par le système d'exploitation. Cependant, pour d'autres contrôles personnalisés, les changements d'état DOIVENT être fournis via les états ARIA tels que aria-checked, aria-disabled, aria-selected, aria-expanded et aria-pressed.</t>
+  </si>
+  <si>
+    <t>Le contenu NE DOIT PAS être limité à une seule orientation, comme le portrait ou le paysage, sauf si cela est essentiel. WCAG 2.1 : Orientation
+    Des exemples de cas où une orientation est essentielle sont une application pour un piano ou un chèque de banque.</t>
+  </si>
+  <si>
+    <t>L'orientation</t>
+  </si>
+  <si>
+    <t>Un titre d'application DOIT être fourni.</t>
+  </si>
+  <si>
     <t>L'ARIA Landmark Roles DOIT être utilisé pour décrire une structure d'application ou de document, telle que banner, complementary, contentinfo, main, navigation, search.</t>
   </si>
   <si>
@@ -600,149 +730,6 @@
   </si>
   <si>
     <t>Les cibles tactiles DOIVENT être suffisamment grandes pour que l'utilisateur puisse interagir avec elles (voir BBC Mobile Accessibility Guidelines pour des directives utiles sur la taille des cibles tactiles).</t>
-  </si>
-  <si>
-    <t>Paramétrer la durée du cache</t>
-  </si>
-  <si>
-    <t>Des erreurs relevées dans le test W3C</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/</t>
-  </si>
-  <si>
-    <t>Le contraste des couleurs DOIT être conforme aux exigences du niveau AA du WCAG 2.1 :
-    Un contraste dont le ratio est de 4.5:1 pour les textes normaux (dont la font est inférieure à 18 points ou 14 points en gras) ;
-    Un contraste dont le ratio est de 3:1 pour les grands textes (18 points minimum ou 14 points en gras).</t>
-  </si>
-  <si>
-    <t>L'attribut "lang" dans le Html doit être renseigné correctement</t>
-  </si>
-  <si>
-    <t>Lighthouse</t>
-  </si>
-  <si>
-    <t>Pas de valeur définie pour les 2 pages</t>
-  </si>
-  <si>
-    <t>Les icônes des réseaux sociaux dans le footer n'ont pas de texte de lien unique et discernable</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/
-Lighthouse</t>
-  </si>
-  <si>
-    <t>Tous les composants de l'interface utilisateur ayant un texte visible (ou une image de texte) comme étiquette (label) DOIVENT avoir le même texte disponible dans le nom programmatique du composant. WCAG 2.1 : Étiquette dans le nom.</t>
-  </si>
-  <si>
-    <t>Des parties de pages comporte un ratio de contraste texte/fond insuffisant</t>
-  </si>
-  <si>
-    <t>Un taux de contraste insuffisant va rendre difficile la lecture pour les personnes mal voyantes.</t>
-  </si>
-  <si>
-    <t>Les éléments interactifs ou cliquables doivent avoir un contenu textuel visible par les lecteurs d'écran</t>
-  </si>
-  <si>
-    <t>Des liens en page 2 n'ont pas de contenu textuel visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le logiciel de lecteur d'écran ne pourra pas restituer à l'utilisateur le contenu et l'intérêt des liens incriminés. </t>
-  </si>
-  <si>
-    <t>Axe Devtools</t>
-  </si>
-  <si>
-    <t>Cela ne facilite pas la compréhension de la page par le lecteur d'ècran et les technologies d'assistance.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page d'accueil, la hierarchie des titres n'est pas correcte. </t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/
-Axe Devtools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il existe des images texte en page accueil sans description adaptée. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le contenu ne pourra pas etre lu par un lecteur d'écran ou une technologie d'assistance. L'utilisateur va passer à coté des informations du site. </t>
-  </si>
-  <si>
-    <t>Des contenus textuels sont lus dans un accent anglais, ce qui rend la compréhension difficile</t>
-  </si>
-  <si>
-    <t>Le formulaire page 2 n'a pas de labels associés. De plus, lors de la lecture d'écran par Voice over, les indications pour chaque inoput sont identiques.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le remplissage du formulaire par l'utilisateur utilisant une technologie d'assistance risque d'être géné par une mauvaise compréhension des éléments. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La structure du code html doit utiliser au maximum les balises sémantiques et être cohérente. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de balise main pour les 2 pages. 
-Un bouton "Toggle navigation" semble errer sans but en haut de la page 2. </t>
-  </si>
-  <si>
-    <t>La navigation en page 2 est à moitié hors écran.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cela ne favorise pas la visibilité de la page et la navigation pour les personnes mal voyantes. </t>
-  </si>
-  <si>
-    <t>Des éléments textuels ne sont pas lus par le lecteur d'écran (voice over). Web design, Stratégie, Illustrations + paragraphes associés. 
-Titres et paragraphes des images en page d'accueil. 
-Paragraphes du bouton envoyer en page 2.</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les liens du footer en page d'accueil n'ont aucune indication de couleur ou autre (à part le pointer de la souris mais les liens sont trop rapporchés entre eux pour que ce pointer soit efficace). </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cela risque de rendre difficile la navigation des personnes mal voyantes. </t>
-  </si>
-  <si>
-    <t>Les éléments  dans le footer sont invisibles en page 2</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/
-Ligthouse
-Wave</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Axe devtools
-Wave</t>
-  </si>
-  <si>
-    <t>https://developer.mozilla.org/
-WCAG - Contrast checker
-Lighthouse
-Wave</t>
-  </si>
-  <si>
-    <t>Version Mobile</t>
-  </si>
-  <si>
-    <t>Lighthouse (version mobile)</t>
-  </si>
-  <si>
-    <t>Rien de plus que la version desktop</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Paramétrer l'attribut " lang" du html avec la version fr.</t>
-  </si>
-  <si>
-    <t>Bien pour les sites statiques mais pas pour les dynamiques</t>
   </si>
 </sst>
 </file>
@@ -895,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -951,23 +938,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1106,9 +1082,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1164,12 +1137,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1202,15 +1196,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1428,11 +1413,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB1019"/>
+  <dimension ref="A1:AB1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19:D20"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1445,9 +1430,9 @@
     <col min="6" max="6" width="48.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="57" customWidth="1"/>
-    <col min="10" max="28" width="10.5703125" style="51" customWidth="1"/>
-    <col min="29" max="16384" width="11.28515625" style="51"/>
+    <col min="9" max="9" width="17.42578125" style="56" customWidth="1"/>
+    <col min="10" max="28" width="10.5703125" style="50" customWidth="1"/>
+    <col min="29" max="16384" width="11.28515625" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1455,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -1478,27 +1463,27 @@
       <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
-      <c r="AA1" s="50"/>
-      <c r="AB1" s="50"/>
-    </row>
-    <row r="2" spans="1:28" s="53" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+    </row>
+    <row r="2" spans="1:28" s="52" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1510,30 +1495,30 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
-      <c r="Z2" s="52"/>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="52"/>
-    </row>
-    <row r="3" spans="1:28" s="55" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+    </row>
+    <row r="3" spans="1:28" s="54" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1542,27 +1527,27 @@
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-    </row>
-    <row r="4" spans="1:28" s="56" customFormat="1" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+    </row>
+    <row r="4" spans="1:28" s="55" customFormat="1" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13" t="s">
@@ -1581,331 +1566,337 @@
         <v>13</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="I4" s="17"/>
     </row>
-    <row r="5" spans="1:28" s="56" customFormat="1" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="55" customFormat="1" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>27</v>
-      </c>
       <c r="G5" s="18" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="1:28" s="56" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="55" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="19"/>
       <c r="C6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="I6" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" s="56" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" s="55" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="19"/>
       <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="H7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="23" t="s">
-        <v>21</v>
-      </c>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:28" s="56" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" s="55" customFormat="1" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="20" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" s="56" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="55" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18"/>
       <c r="B9" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="25"/>
       <c r="D9" s="25" t="s">
-        <v>29</v>
+        <v>181</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="25"/>
       <c r="H9" s="26"/>
       <c r="I9" s="27"/>
     </row>
-    <row r="10" spans="1:28" s="56" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
+    <row r="10" spans="1:28" s="55" customFormat="1" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="76"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="78" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="71" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="70" t="s">
-        <v>110</v>
-      </c>
-      <c r="G10" s="70" t="s">
-        <v>107</v>
+      <c r="C10" s="84" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>98</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" s="56" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="79"/>
+        <v>28</v>
+      </c>
+      <c r="I10" s="63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" s="55" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="85"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="78"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
       <c r="H11" s="23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="79"/>
+    <row r="12" spans="1:28" s="55" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="85"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
       <c r="H12" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" s="55" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="78"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="76"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="23" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:28" s="56" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" s="55" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="70"/>
-      <c r="G14" s="70"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
       <c r="H14" s="23" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="I14" s="29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" s="56" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" s="55" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="78"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="23" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="I15" s="22"/>
     </row>
-    <row r="16" spans="1:28" s="56" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" s="55" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
       <c r="H16" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="22"/>
-    </row>
-    <row r="17" spans="1:9" s="56" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="70"/>
+        <v>46</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="55" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="76"/>
       <c r="B17" s="19"/>
-      <c r="C17" s="78" t="s">
+      <c r="C17" s="84" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="83" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="1:9" s="55" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="85"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17" s="77" t="s">
-        <v>107</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="1:9" s="56" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="79"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="77"/>
+      <c r="G18" s="83"/>
       <c r="H18" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I18" s="30"/>
     </row>
-    <row r="19" spans="1:9" s="56" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="55" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18"/>
       <c r="B19" s="19"/>
-      <c r="C19" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="70" t="s">
-        <v>213</v>
-      </c>
-      <c r="E19" s="70"/>
+      <c r="C19" s="84" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="E19" s="76" t="s">
+        <v>186</v>
+      </c>
       <c r="F19" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="G19" s="70"/>
+        <v>96</v>
+      </c>
+      <c r="G19" s="76" t="s">
+        <v>177</v>
+      </c>
       <c r="H19" s="23" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="I19" s="22"/>
     </row>
-    <row r="20" spans="1:9" s="56" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="55" customFormat="1" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18"/>
       <c r="B20" s="19"/>
-      <c r="C20" s="78"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
       <c r="F20" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="G20" s="70"/>
+        <v>47</v>
+      </c>
+      <c r="G20" s="76"/>
       <c r="H20" s="21" t="s">
-        <v>171</v>
+        <v>145</v>
       </c>
       <c r="I20" s="22"/>
     </row>
-    <row r="21" spans="1:9" s="56" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="55" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18"/>
       <c r="B21" s="19"/>
       <c r="C21" s="20" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>116</v>
+        <v>187</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="I21" s="30"/>
     </row>
-    <row r="22" spans="1:9" s="56" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="55" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="31"/>
@@ -1915,382 +1906,380 @@
       <c r="H22" s="32"/>
       <c r="I22" s="33"/>
     </row>
-    <row r="23" spans="1:9" s="58" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="57" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="34"/>
       <c r="B23" s="35"/>
       <c r="C23" s="20" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G23" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="H23" s="69" t="s">
-        <v>212</v>
-      </c>
-      <c r="I23" s="67" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="58" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+      <c r="H23" s="68" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="66" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="57" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="34"/>
       <c r="B24" s="35"/>
       <c r="C24" s="20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G24" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="58" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="57" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
-      <c r="C25" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="73" t="s">
-        <v>80</v>
+      <c r="C25" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="79" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="79" t="s">
+        <v>75</v>
       </c>
       <c r="F25" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G25" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="H25" s="74" t="s">
-        <v>120</v>
-      </c>
-      <c r="I25" s="72" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="58" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="G25" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="80" t="s">
+        <v>109</v>
+      </c>
+      <c r="I25" s="78" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="57" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="34"/>
       <c r="B26" s="35"/>
-      <c r="C26" s="78"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="73"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
       <c r="F26" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="G26" s="76"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="73"/>
-    </row>
-    <row r="27" spans="1:9" s="58" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="G26" s="82"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="79"/>
+    </row>
+    <row r="27" spans="1:9" s="57" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="34"/>
       <c r="B27" s="35"/>
-      <c r="C27" s="78"/>
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
       <c r="F27" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G27" s="76"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="73"/>
-    </row>
-    <row r="28" spans="1:9" s="58" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="G27" s="82"/>
+      <c r="H27" s="81"/>
+      <c r="I27" s="79"/>
+    </row>
+    <row r="28" spans="1:9" s="57" customFormat="1" ht="86" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="34"/>
       <c r="B28" s="35"/>
-      <c r="C28" s="78"/>
-      <c r="D28" s="73"/>
-      <c r="E28" s="73"/>
+      <c r="C28" s="84"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
       <c r="F28" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" s="76"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="73"/>
-    </row>
-    <row r="29" spans="1:9" s="58" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+      <c r="G28" s="82"/>
+      <c r="H28" s="81"/>
+      <c r="I28" s="79"/>
+    </row>
+    <row r="29" spans="1:9" s="57" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="34"/>
       <c r="B29" s="35"/>
       <c r="C29" s="20" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="16" t="s">
-        <v>131</v>
+        <v>189</v>
       </c>
       <c r="I29" s="30"/>
     </row>
-    <row r="30" spans="1:9" s="58" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" s="57" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="34"/>
       <c r="B30" s="35"/>
       <c r="C30" s="20" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>96</v>
+        <v>190</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="I30" s="36"/>
     </row>
-    <row r="31" spans="1:9" s="58" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" s="57" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="34"/>
       <c r="B31" s="35"/>
       <c r="C31" s="20" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>99</v>
+        <v>182</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="H31" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="I31" s="17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="56" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9" s="55" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
       <c r="C32" s="20" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>16</v>
+        <v>178</v>
       </c>
       <c r="H32" s="23" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="I32" s="22"/>
     </row>
-    <row r="33" spans="1:9" s="56" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="55" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="19"/>
       <c r="C33" s="39" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H33" s="16" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="I33" s="40"/>
     </row>
-    <row r="34" spans="1:9" s="56" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="55" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="19"/>
       <c r="C34" s="39" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D34" s="19" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>86</v>
+        <v>191</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="H34" s="23" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="I34" s="41"/>
     </row>
-    <row r="35" spans="1:9" s="56" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" s="55" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="19"/>
       <c r="C35" s="39" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>138</v>
+        <v>192</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H35" s="14" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="I35" s="30"/>
     </row>
-    <row r="36" spans="1:9" s="56" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" s="55" customFormat="1" ht="71" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="39" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>144</v>
+        <v>193</v>
       </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" s="56" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" s="55" customFormat="1" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
       <c r="C37" s="39" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D37" s="14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="I37" s="30"/>
     </row>
-    <row r="38" spans="1:9" s="56" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" s="55" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="19"/>
       <c r="C38" s="39" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="I38" s="64" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="56" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+      <c r="I38" s="63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="55" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
       <c r="C39" s="39" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G39" s="14" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="56" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="55" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B40" s="43"/>
       <c r="C40" s="43"/>
@@ -2301,397 +2290,365 @@
       <c r="H40" s="43"/>
       <c r="I40" s="44"/>
     </row>
-    <row r="41" spans="1:9" s="56" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" s="55" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="19"/>
-      <c r="C41" s="80" t="s">
-        <v>149</v>
-      </c>
-      <c r="D41" s="59" t="s">
-        <v>181</v>
-      </c>
-      <c r="E41" s="62" t="s">
-        <v>182</v>
+      <c r="C41" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="58" t="s">
+        <v>195</v>
+      </c>
+      <c r="E41" s="61" t="s">
+        <v>153</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>174</v>
-      </c>
-      <c r="G41" s="49" t="s">
-        <v>207</v>
-      </c>
-      <c r="H41" s="19"/>
-      <c r="I41" s="22"/>
-    </row>
-    <row r="42" spans="1:9" s="56" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="G41" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="I41" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" s="55" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="19"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="62" t="s">
-        <v>201</v>
-      </c>
-      <c r="E42" s="62" t="s">
-        <v>202</v>
+      <c r="C42" s="86"/>
+      <c r="D42" s="61" t="s">
+        <v>196</v>
+      </c>
+      <c r="E42" s="61" t="s">
+        <v>166</v>
       </c>
       <c r="F42" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="G42" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="H42" s="19"/>
+        <v>138</v>
+      </c>
+      <c r="G42" s="48" t="s">
+        <v>147</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>203</v>
+      </c>
       <c r="I42" s="22"/>
     </row>
-    <row r="43" spans="1:9" s="56" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" s="55" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="19"/>
-      <c r="C43" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="D43" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="E43" s="65" t="s">
-        <v>198</v>
+      <c r="C43" s="86" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="64" t="s">
+        <v>164</v>
       </c>
       <c r="F43" s="46" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="H43" s="37"/>
       <c r="I43" s="30"/>
     </row>
-    <row r="44" spans="1:9" s="56" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" s="55" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="19"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="60" t="s">
-        <v>203</v>
-      </c>
-      <c r="E44" s="65" t="s">
-        <v>202</v>
+      <c r="C44" s="86"/>
+      <c r="D44" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="64" t="s">
+        <v>166</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>158</v>
-      </c>
-      <c r="G44" s="66" t="s">
-        <v>204</v>
+        <v>140</v>
+      </c>
+      <c r="G44" s="65" t="s">
+        <v>168</v>
       </c>
       <c r="H44" s="37"/>
       <c r="I44" s="30"/>
     </row>
-    <row r="45" spans="1:9" s="56" customFormat="1" ht="119" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="19"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="81" t="s">
-        <v>151</v>
-      </c>
-      <c r="D45" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="45" t="s">
-        <v>159</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H45" s="19"/>
-      <c r="I45" s="22"/>
-    </row>
-    <row r="46" spans="1:9" s="56" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="82"/>
-      <c r="D46" s="62" t="s">
-        <v>200</v>
-      </c>
-      <c r="E46" s="19"/>
-      <c r="F46" s="45" t="s">
-        <v>160</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H46" s="19"/>
-      <c r="I46" s="22"/>
-    </row>
-    <row r="47" spans="1:9" s="56" customFormat="1" ht="131" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" s="55" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="73"/>
+      <c r="B45" s="73"/>
+      <c r="C45" s="87" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45" s="75"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="46" t="s">
+        <v>205</v>
+      </c>
+      <c r="G45" s="65"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="30"/>
+    </row>
+    <row r="46" spans="1:9" s="55" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="73"/>
+      <c r="B46" s="73"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="75"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="G46" s="65"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="30"/>
+    </row>
+    <row r="47" spans="1:9" s="55" customFormat="1" ht="131" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="19"/>
-      <c r="C47" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="D47" s="60" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" s="37"/>
+      <c r="C47" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="59" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="69" t="s">
+        <v>197</v>
+      </c>
       <c r="F47" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="G47" s="49" t="s">
-        <v>179</v>
-      </c>
-      <c r="H47" s="37"/>
+        <v>141</v>
+      </c>
+      <c r="G47" s="48" t="s">
+        <v>151</v>
+      </c>
+      <c r="H47" s="37" t="s">
+        <v>175</v>
+      </c>
       <c r="I47" s="30"/>
     </row>
-    <row r="48" spans="1:9" s="56" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" s="55" customFormat="1" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="19"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="65" t="s">
-        <v>190</v>
-      </c>
-      <c r="E48" s="65" t="s">
-        <v>191</v>
+      <c r="C48" s="86"/>
+      <c r="D48" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="64" t="s">
+        <v>197</v>
       </c>
       <c r="F48" s="46" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="H48" s="37"/>
       <c r="I48" s="17"/>
     </row>
-    <row r="49" spans="1:9" s="56" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="63"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="65" t="s">
-        <v>184</v>
-      </c>
-      <c r="E49" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="F49" s="65" t="s">
-        <v>183</v>
-      </c>
-      <c r="G49" s="66" t="s">
-        <v>206</v>
+    <row r="49" spans="1:9" s="55" customFormat="1" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="62"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="86"/>
+      <c r="D49" s="64" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="F49" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="G49" s="65" t="s">
+        <v>169</v>
       </c>
       <c r="H49" s="37"/>
       <c r="I49" s="30"/>
     </row>
-    <row r="50" spans="1:9" s="56" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" s="55" customFormat="1" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="19"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="65" t="s">
-        <v>199</v>
-      </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="60" t="s">
-        <v>180</v>
+      <c r="C50" s="86"/>
+      <c r="D50" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="F50" s="59" t="s">
+        <v>152</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="H50" s="37"/>
       <c r="I50" s="17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="56" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="55" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="19"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="60" t="s">
-        <v>193</v>
-      </c>
-      <c r="E51" s="65" t="s">
-        <v>194</v>
+      <c r="C51" s="86"/>
+      <c r="D51" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="E51" s="64" t="s">
+        <v>160</v>
       </c>
       <c r="F51" s="46" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="H51" s="37"/>
       <c r="I51" s="30"/>
     </row>
-    <row r="52" spans="1:9" s="56" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="19"/>
-      <c r="B52" s="19"/>
-      <c r="C52" s="47" t="s">
-        <v>153</v>
-      </c>
-      <c r="D52" s="62" t="s">
-        <v>205</v>
-      </c>
-      <c r="E52" s="19"/>
-      <c r="F52" s="45" t="s">
-        <v>164</v>
-      </c>
-      <c r="G52" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H52" s="19"/>
-      <c r="I52" s="22"/>
-    </row>
-    <row r="53" spans="1:9" s="56" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="19"/>
-      <c r="B53" s="19"/>
-      <c r="C53" s="47" t="s">
-        <v>154</v>
-      </c>
-      <c r="D53" s="65" t="s">
-        <v>200</v>
-      </c>
-      <c r="E53" s="37"/>
+    <row r="52" spans="1:9" s="55" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="73"/>
+      <c r="B52" s="73"/>
+      <c r="C52" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="D52" s="75"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="G52" s="73"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="30"/>
+    </row>
+    <row r="53" spans="1:9" s="55" customFormat="1" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="73"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="D53" s="75"/>
+      <c r="E53" s="75"/>
       <c r="F53" s="46" t="s">
-        <v>165</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>173</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="G53" s="73"/>
       <c r="H53" s="37"/>
       <c r="I53" s="30"/>
     </row>
-    <row r="54" spans="1:9" s="56" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="63"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="83" t="s">
-        <v>208</v>
-      </c>
-      <c r="D54" s="65" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="62" t="s">
-        <v>209</v>
-      </c>
-      <c r="H54" s="37"/>
-      <c r="I54" s="30"/>
-    </row>
-    <row r="55" spans="1:9" ht="234" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="48"/>
-      <c r="B55" s="48"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="45" t="s">
-        <v>169</v>
-      </c>
-      <c r="G55" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="H55" s="48"/>
-      <c r="I55" s="22"/>
-    </row>
-    <row r="56" spans="1:9" ht="76" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="48"/>
-      <c r="B56" s="48"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="48"/>
-      <c r="E56" s="48"/>
+    <row r="54" spans="1:9" s="55" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="60"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="86" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="58" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="F54" s="58" t="s">
+        <v>149</v>
+      </c>
+      <c r="G54" s="58" t="s">
+        <v>150</v>
+      </c>
+      <c r="H54" s="60"/>
+      <c r="I54" s="63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="55" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="73"/>
+      <c r="B55" s="73"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="G55" s="72"/>
+      <c r="H55" s="73"/>
+      <c r="I55" s="74"/>
+    </row>
+    <row r="56" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="47"/>
+      <c r="B56" s="47"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" s="67" t="s">
+        <v>200</v>
+      </c>
       <c r="F56" s="45" t="s">
-        <v>170</v>
-      </c>
-      <c r="G56" s="63" t="s">
-        <v>173</v>
-      </c>
-      <c r="H56" s="48"/>
+        <v>144</v>
+      </c>
+      <c r="G56" s="48" t="s">
+        <v>157</v>
+      </c>
+      <c r="H56" s="47"/>
       <c r="I56" s="22"/>
     </row>
-    <row r="57" spans="1:9" s="56" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19"/>
-      <c r="B57" s="19"/>
-      <c r="C57" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="D57" s="62" t="s">
+    <row r="57" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="47"/>
+      <c r="B57" s="47"/>
+      <c r="C57" s="86"/>
+      <c r="D57" s="67"/>
+      <c r="E57" s="67"/>
+      <c r="F57" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="G57" s="48"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="22"/>
+    </row>
+    <row r="58" spans="1:9" ht="230" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="47"/>
+      <c r="B58" s="47"/>
+      <c r="C58" s="86"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="67"/>
+      <c r="F58" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="G58" s="48"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="22"/>
+    </row>
+    <row r="59" spans="1:9" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="47"/>
+      <c r="B59" s="47"/>
+      <c r="C59" s="86"/>
+      <c r="D59" s="67"/>
+      <c r="E59" s="67"/>
+      <c r="F59" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="G59" s="48"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="22"/>
+    </row>
+    <row r="60" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="47"/>
+      <c r="B60" s="47"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="67" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" s="67" t="s">
         <v>200</v>
       </c>
-      <c r="E57" s="19"/>
-      <c r="F57" s="45" t="s">
-        <v>166</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H57" s="19"/>
-      <c r="I57" s="22"/>
-    </row>
-    <row r="58" spans="1:9" s="56" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="61"/>
-      <c r="B58" s="61"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="59" t="s">
-        <v>177</v>
-      </c>
-      <c r="E58" s="62" t="s">
-        <v>192</v>
-      </c>
-      <c r="F58" s="59" t="s">
-        <v>175</v>
-      </c>
-      <c r="G58" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="H58" s="61"/>
-      <c r="I58" s="64" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="48"/>
-      <c r="B59" s="48"/>
-      <c r="C59" s="80"/>
-      <c r="D59" s="68" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" s="68" t="s">
-        <v>187</v>
-      </c>
-      <c r="F59" s="45" t="s">
-        <v>167</v>
-      </c>
-      <c r="G59" s="49" t="s">
-        <v>189</v>
-      </c>
-      <c r="H59" s="48"/>
-      <c r="I59" s="22"/>
-    </row>
-    <row r="60" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="48"/>
-      <c r="B60" s="48"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="68" t="s">
-        <v>196</v>
-      </c>
-      <c r="E60" s="68" t="s">
-        <v>187</v>
-      </c>
-      <c r="F60" s="62" t="s">
-        <v>195</v>
-      </c>
-      <c r="G60" s="62" t="s">
-        <v>186</v>
-      </c>
-      <c r="H60" s="48"/>
+      <c r="F60" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="G60" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="H60" s="47"/>
       <c r="I60" s="22"/>
     </row>
-    <row r="61" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="48"/>
-      <c r="B61" s="48"/>
-      <c r="C61" s="80"/>
-      <c r="D61" s="68" t="s">
-        <v>205</v>
-      </c>
-      <c r="E61" s="48"/>
-      <c r="F61" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="H61" s="48"/>
-      <c r="I61" s="22"/>
-    </row>
+    <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3649,15 +3606,13 @@
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="24">
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C47:C51"/>
+    <mergeCell ref="C54:C60"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C51"/>
-    <mergeCell ref="C57:C61"/>
-    <mergeCell ref="C54:C56"/>
     <mergeCell ref="C25:C28"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A17:A18"/>
@@ -3685,7 +3640,7 @@
     <hyperlink ref="G43" r:id="rId4" xr:uid="{C0BA0263-F2C5-B341-A3C1-B103392E559D}"/>
     <hyperlink ref="G47" r:id="rId5" xr:uid="{08AB339A-4389-0049-AF0A-0206FA32EC6E}"/>
     <hyperlink ref="G44" r:id="rId6" xr:uid="{5E968017-85F5-014E-A2D1-93777B2C5CA6}"/>
-    <hyperlink ref="G59" r:id="rId7" xr:uid="{3DE14659-F789-6B40-A824-F9B5019B2358}"/>
+    <hyperlink ref="G56" r:id="rId7" xr:uid="{3DE14659-F789-6B40-A824-F9B5019B2358}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>